<commit_message>
modifies login test 001 and 002
</commit_message>
<xml_diff>
--- a/src/test/java/com/koinpro/testData/Koinpro_Testcases.xlsx
+++ b/src/test/java/com/koinpro/testData/Koinpro_Testcases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="42">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -601,7 +601,7 @@
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H3"/>
     </row>

</xml_diff>